<commit_message>
[Doc] update "TABLE.xlsx", doc history
</commit_message>
<xml_diff>
--- a/doc/TABLE.xlsx
+++ b/doc/TABLE.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="11895"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="테이블" sheetId="1" r:id="rId1"/>
     <sheet name="변경내용" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>내용</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,42 +81,209 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">		Duty(String)</t>
+  </si>
+  <si>
+    <t>(간격:반복:알림예시)3:3:3,7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlarmCycle(int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복 주기(분:1~60)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlarmMaxCount(int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복 횟수(회:0~99)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlarmNotice(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">		DayCircle(String)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMNOTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(80)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">		AlarmNote(String)</t>
+  </si>
+  <si>
+    <t>알람 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FILENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">		FileName(String)</t>
+  </si>
+  <si>
+    <t>알람 파일 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIBELEVEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">		VibeLevle(int)</t>
+  </si>
+  <si>
+    <t>알람 진동 세기(0~10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMCOUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">		AlarmCount(int)</t>
+  </si>
+  <si>
+    <t>현재 알람울린횟수(회:0~99)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정/변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤혜정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DUTY 분할</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DUTY 분할</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분할 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 포맷 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAYCIRCLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COLUMN 명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COLUMN TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림 일자 (0 ~ xx,yy,zz : xx일전, yy일전, zz일전)</t>
+  </si>
+  <si>
+    <t>변수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TABLE명 : ALARM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서 수정내역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤혜정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.09.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>DUTY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">		Duty(String)</t>
-  </si>
-  <si>
-    <t>(간격:반복:알림예시)3:3:3,7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NUMBER(2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlarmCycle(int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>반복 주기(분:1~60)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlarmMaxCount(int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>반복 횟수(회:0~99)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlarmNotice(String)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">		DayCircle(String)</t>
+    <t>ALARMCYCLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMMAXCOUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMNOTICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAYCIRCLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -124,165 +291,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ALARMNOTE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(80)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">		AlarmNote(String)</t>
-  </si>
-  <si>
-    <t>알람 내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FILENAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(40)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">		FileName(String)</t>
-  </si>
-  <si>
-    <t>알람 파일 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VIBELEVEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">		VibeLevle(int)</t>
-  </si>
-  <si>
-    <t>알람 진동 세기(0~10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMCOUNT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">		AlarmCount(int)</t>
-  </si>
-  <si>
-    <t>현재 알람울린횟수(회:0~99)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정/변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>변경자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>변경날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>윤혜정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>변경내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DUTY 분할</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DUTY 분할</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>분할 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 포맷 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMCYCLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NUMBER(2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMMAXCOUNT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMNOTICE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAYCIRCLE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR2(7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COLUMN 명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COLUMN TYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알림 일자 (0 ~ xx,yy,zz : xx일전, yy일전, zz일전)</t>
-  </si>
-  <si>
     <t>요일반복 (0101010 : 일/월/화/수/목/금/토, 0:비활성 1:활성)</t>
-  </si>
-  <si>
-    <t>변수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TABLE명 : ALARM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">일부 데이터 포맷 삭제 및 변경
+    - DUTY 삭제, ALARMCYCLE, ALARMMAXCOUNT, ALARMNOTICE 분할
+    - DAYCIRCLE 포맷 변경 0,1,0,1,0,1,0//일,월,화,수,목,금,토 -&gt; 0101010 : 일/월/화/수/목/금/토
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경 인덱스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,6 : 삭제
+11, 12, 13, 14 : 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +366,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -415,13 +460,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -463,6 +530,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +644,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -588,7 +678,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -764,14 +853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
@@ -781,41 +870,41 @@
     <col min="10" max="10" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="18" thickBot="1">
       <c r="B2" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="18" thickBot="1">
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="J3" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -836,7 +925,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12">
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -857,7 +946,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -878,7 +967,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -899,259 +988,259 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12">
       <c r="B8" s="5">
         <v>5</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="G8" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" s="12">
         <v>20190922</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="4">
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="12">
         <v>20190922</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="5">
         <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="F10" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12">
       <c r="B11" s="4">
         <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="F11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12">
       <c r="B12" s="5">
         <v>9</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12">
       <c r="B13" s="4">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12">
       <c r="B14" s="5">
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2">
         <v>20190922</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12">
       <c r="B15" s="4">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I15" s="2">
         <v>20190922</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="5">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I16" s="2">
         <v>20190922</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="4">
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="2">
         <v>20190922</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1162,14 +1251,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="97.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+    </row>
+    <row r="2" spans="2:5" ht="18" thickBot="1">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="2:5" ht="18" thickBot="1">
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="69">
+      <c r="B4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>